<commit_message>
Agregar un producto listo
</commit_message>
<xml_diff>
--- a/assets/admin/template-files/importar_productos.xlsx
+++ b/assets/admin/template-files/importar_productos.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Modelo</t>
   </si>
   <si>
-    <t xml:space="preserve">Descripción</t>
+    <t xml:space="preserve">Impresoras</t>
   </si>
   <si>
     <t xml:space="preserve">Color</t>
@@ -289,9 +289,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>10440</xdr:colOff>
+      <xdr:colOff>10080</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>807840</xdr:rowOff>
+      <xdr:rowOff>807480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -304,8 +304,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5415480" y="2166480"/>
-          <a:ext cx="947880" cy="753120"/>
+          <a:off x="5329800" y="2166480"/>
+          <a:ext cx="928440" cy="752760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -326,9 +326,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>722880</xdr:colOff>
+      <xdr:colOff>722520</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>825480</xdr:rowOff>
+      <xdr:rowOff>825120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -341,8 +341,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5473080" y="344880"/>
-          <a:ext cx="621720" cy="795240"/>
+          <a:off x="5387400" y="344880"/>
+          <a:ext cx="621360" cy="794880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -363,9 +363,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>717120</xdr:colOff>
+      <xdr:colOff>716760</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>814320</xdr:rowOff>
+      <xdr:rowOff>813960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -378,8 +378,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5483520" y="1266120"/>
-          <a:ext cx="605520" cy="761400"/>
+          <a:off x="5397840" y="1266120"/>
+          <a:ext cx="605160" cy="761040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -407,15 +407,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>